<commit_message>
Added README, filled in BOM to provide order list for DIGIKEY
</commit_message>
<xml_diff>
--- a/UWED2_proto.xlsx
+++ b/UWED2_proto.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mdeweerd\KiCAD\uwed-kicad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E0F869-B09A-4903-BB10-6AFF7A2AC8BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="^_ana.neg5_micro1_micro2_reg1_r" sheetId="1" r:id="rId1"/>
@@ -21,17 +27,17 @@
     <definedName name="tme_part_data">'^_ana.neg5_micro1_micro2_reg1_r'!$AS$5:$AW$32</definedName>
     <definedName name="TotalCost">'^_ana.neg5_micro1_micro2_reg1_r'!$N$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC3" authorId="0">
+    <comment ref="AC3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH3" authorId="0">
+    <comment ref="AH3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM3" authorId="0">
+    <comment ref="AM3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR3" authorId="0">
+    <comment ref="AR3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW3" authorId="0">
+    <comment ref="AW3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -135,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -148,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -174,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -187,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -200,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -213,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -226,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -239,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -252,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -265,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -279,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0">
+    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -296,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="0">
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -309,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="0">
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -322,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="0">
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -337,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="0">
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -352,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q6" authorId="0">
+    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -366,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R6" authorId="0">
+    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -381,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S6" authorId="0">
+    <comment ref="S6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -394,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T6" authorId="0">
+    <comment ref="T6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -409,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U6" authorId="0">
+    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -424,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V6" authorId="0">
+    <comment ref="V6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -438,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W6" authorId="0">
+    <comment ref="W6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -453,7 +459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X6" authorId="0">
+    <comment ref="X6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -466,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y6" authorId="0">
+    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -481,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z6" authorId="0">
+    <comment ref="Z6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
       <text>
         <r>
           <rPr>
@@ -496,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA6" authorId="0">
+    <comment ref="AA6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
       <text>
         <r>
           <rPr>
@@ -510,7 +516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB6" authorId="0">
+    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -525,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC6" authorId="0">
+    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -538,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD6" authorId="0">
+    <comment ref="AD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -553,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE6" authorId="0">
+    <comment ref="AE6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -568,7 +574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF6" authorId="0">
+    <comment ref="AF6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -582,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG6" authorId="0">
+    <comment ref="AG6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
       <text>
         <r>
           <rPr>
@@ -597,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH6" authorId="0">
+    <comment ref="AH6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -610,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI6" authorId="0">
+    <comment ref="AI6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -625,7 +631,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ6" authorId="0">
+    <comment ref="AJ6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -640,7 +646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK6" authorId="0">
+    <comment ref="AK6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -654,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL6" authorId="0">
+    <comment ref="AL6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -669,7 +675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="0">
+    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -682,7 +688,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="0">
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
       <text>
         <r>
           <rPr>
@@ -697,7 +703,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
       <text>
         <r>
           <rPr>
@@ -712,7 +718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
       <text>
         <r>
           <rPr>
@@ -726,7 +732,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000033000000}">
       <text>
         <r>
           <rPr>
@@ -741,7 +747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="0">
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000034000000}">
       <text>
         <r>
           <rPr>
@@ -754,7 +760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0">
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000035000000}">
       <text>
         <r>
           <rPr>
@@ -769,7 +775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000036000000}">
       <text>
         <r>
           <rPr>
@@ -784,7 +790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000037000000}">
       <text>
         <r>
           <rPr>
@@ -798,7 +804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000038000000}">
       <text>
         <r>
           <rPr>
@@ -813,7 +819,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000039000000}">
       <text>
         <r>
           <rPr>
@@ -826,7 +832,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q7" authorId="0">
+    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -855,7 +861,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V7" authorId="0">
+    <comment ref="V7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -879,7 +885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y7" authorId="0">
+    <comment ref="Y7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -892,7 +898,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA7" authorId="0">
+    <comment ref="AA7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -914,7 +920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF7" authorId="0">
+    <comment ref="AF7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -935,7 +941,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK7" authorId="0">
+    <comment ref="AK7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003F000000}">
       <text>
         <r>
           <rPr>
@@ -958,7 +964,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP7" authorId="0">
+    <comment ref="AP7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000040000000}">
       <text>
         <r>
           <rPr>
@@ -980,7 +986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0">
+    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000041000000}">
       <text>
         <r>
           <rPr>
@@ -1000,7 +1006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T8" authorId="0">
+    <comment ref="T8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000042000000}">
       <text>
         <r>
           <rPr>
@@ -1013,7 +1019,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V8" authorId="0">
+    <comment ref="V8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000043000000}">
       <text>
         <r>
           <rPr>
@@ -1030,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y8" authorId="0">
+    <comment ref="Y8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000044000000}">
       <text>
         <r>
           <rPr>
@@ -1043,7 +1049,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA8" authorId="0">
+    <comment ref="AA8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000045000000}">
       <text>
         <r>
           <rPr>
@@ -1067,7 +1073,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI8" authorId="0">
+    <comment ref="AI8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000046000000}">
       <text>
         <r>
           <rPr>
@@ -1080,7 +1086,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU8" authorId="0">
+    <comment ref="AU8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000047000000}">
       <text>
         <r>
           <rPr>
@@ -1101,7 +1107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="0">
+    <comment ref="Q9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000048000000}">
       <text>
         <r>
           <rPr>
@@ -1121,7 +1127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V9" authorId="0">
+    <comment ref="V9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000049000000}">
       <text>
         <r>
           <rPr>
@@ -1144,7 +1150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA9" authorId="0">
+    <comment ref="AA9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004A000000}">
       <text>
         <r>
           <rPr>
@@ -1168,7 +1174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF9" authorId="0">
+    <comment ref="AF9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004B000000}">
       <text>
         <r>
           <rPr>
@@ -1189,7 +1195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK9" authorId="0">
+    <comment ref="AK9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004C000000}">
       <text>
         <r>
           <rPr>
@@ -1214,7 +1220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP9" authorId="0">
+    <comment ref="AP9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004D000000}">
       <text>
         <r>
           <rPr>
@@ -1238,7 +1244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU9" authorId="0">
+    <comment ref="AU9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004E000000}">
       <text>
         <r>
           <rPr>
@@ -1259,7 +1265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q10" authorId="0">
+    <comment ref="Q10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004F000000}">
       <text>
         <r>
           <rPr>
@@ -1279,7 +1285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V10" authorId="0">
+    <comment ref="V10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000050000000}">
       <text>
         <r>
           <rPr>
@@ -1302,7 +1308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA10" authorId="0">
+    <comment ref="AA10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000051000000}">
       <text>
         <r>
           <rPr>
@@ -1323,7 +1329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF10" authorId="0">
+    <comment ref="AF10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000052000000}">
       <text>
         <r>
           <rPr>
@@ -1344,7 +1350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q11" authorId="0">
+    <comment ref="Q11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000053000000}">
       <text>
         <r>
           <rPr>
@@ -1364,7 +1370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V11" authorId="0">
+    <comment ref="V11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000054000000}">
       <text>
         <r>
           <rPr>
@@ -1387,7 +1393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN11" authorId="0">
+    <comment ref="AN11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000055000000}">
       <text>
         <r>
           <rPr>
@@ -1400,7 +1406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP11" authorId="0">
+    <comment ref="AP11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000056000000}">
       <text>
         <r>
           <rPr>
@@ -1421,7 +1427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU11" authorId="0">
+    <comment ref="AU11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000057000000}">
       <text>
         <r>
           <rPr>
@@ -1442,7 +1448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q12" authorId="0">
+    <comment ref="Q12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000058000000}">
       <text>
         <r>
           <rPr>
@@ -1461,7 +1467,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V12" authorId="0">
+    <comment ref="V12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000059000000}">
       <text>
         <r>
           <rPr>
@@ -1484,7 +1490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y12" authorId="0">
+    <comment ref="Y12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005A000000}">
       <text>
         <r>
           <rPr>
@@ -1497,7 +1503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA12" authorId="0">
+    <comment ref="AA12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005B000000}">
       <text>
         <r>
           <rPr>
@@ -1521,7 +1527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD12" authorId="0">
+    <comment ref="AD12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005C000000}">
       <text>
         <r>
           <rPr>
@@ -1534,7 +1540,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF12" authorId="0">
+    <comment ref="AF12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005D000000}">
       <text>
         <r>
           <rPr>
@@ -1555,7 +1561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI12" authorId="0">
+    <comment ref="AI12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005E000000}">
       <text>
         <r>
           <rPr>
@@ -1568,7 +1574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK12" authorId="0">
+    <comment ref="AK12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005F000000}">
       <text>
         <r>
           <rPr>
@@ -1593,7 +1599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP12" authorId="0">
+    <comment ref="AP12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000060000000}">
       <text>
         <r>
           <rPr>
@@ -1612,7 +1618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS12" authorId="0">
+    <comment ref="AS12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000061000000}">
       <text>
         <r>
           <rPr>
@@ -1625,7 +1631,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU12" authorId="0">
+    <comment ref="AU12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000062000000}">
       <text>
         <r>
           <rPr>
@@ -1644,7 +1650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q13" authorId="0">
+    <comment ref="Q13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000063000000}">
       <text>
         <r>
           <rPr>
@@ -1660,7 +1666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V13" authorId="0">
+    <comment ref="V13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000064000000}">
       <text>
         <r>
           <rPr>
@@ -1681,7 +1687,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF13" authorId="0">
+    <comment ref="AF13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000065000000}">
       <text>
         <r>
           <rPr>
@@ -1702,7 +1708,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK13" authorId="0">
+    <comment ref="AK13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000066000000}">
       <text>
         <r>
           <rPr>
@@ -1722,7 +1728,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V14" authorId="0">
+    <comment ref="V14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000067000000}">
       <text>
         <r>
           <rPr>
@@ -1739,7 +1745,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF14" authorId="0">
+    <comment ref="AF14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000068000000}">
       <text>
         <r>
           <rPr>
@@ -1760,7 +1766,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q15" authorId="0">
+    <comment ref="Q15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000069000000}">
       <text>
         <r>
           <rPr>
@@ -1779,7 +1785,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V15" authorId="0">
+    <comment ref="V15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006A000000}">
       <text>
         <r>
           <rPr>
@@ -1798,7 +1804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA15" authorId="0">
+    <comment ref="AA15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006B000000}">
       <text>
         <r>
           <rPr>
@@ -1819,7 +1825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF15" authorId="0">
+    <comment ref="AF15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006C000000}">
       <text>
         <r>
           <rPr>
@@ -1840,7 +1846,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP15" authorId="0">
+    <comment ref="AP15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006D000000}">
       <text>
         <r>
           <rPr>
@@ -1860,7 +1866,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q16" authorId="0">
+    <comment ref="Q16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006E000000}">
       <text>
         <r>
           <rPr>
@@ -1884,7 +1890,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V16" authorId="0">
+    <comment ref="V16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006F000000}">
       <text>
         <r>
           <rPr>
@@ -1904,7 +1910,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y16" authorId="0">
+    <comment ref="Y16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000070000000}">
       <text>
         <r>
           <rPr>
@@ -1917,7 +1923,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA16" authorId="0">
+    <comment ref="AA16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000071000000}">
       <text>
         <r>
           <rPr>
@@ -1939,7 +1945,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF16" authorId="0">
+    <comment ref="AF16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000072000000}">
       <text>
         <r>
           <rPr>
@@ -1960,7 +1966,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP16" authorId="0">
+    <comment ref="AP16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000073000000}">
       <text>
         <r>
           <rPr>
@@ -1981,7 +1987,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU16" authorId="0">
+    <comment ref="AU16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000074000000}">
       <text>
         <r>
           <rPr>
@@ -2000,7 +2006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q17" authorId="0">
+    <comment ref="Q17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000075000000}">
       <text>
         <r>
           <rPr>
@@ -2022,7 +2028,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V17" authorId="0">
+    <comment ref="V17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000076000000}">
       <text>
         <r>
           <rPr>
@@ -2041,7 +2047,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA17" authorId="0">
+    <comment ref="AA17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000077000000}">
       <text>
         <r>
           <rPr>
@@ -2062,7 +2068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF17" authorId="0">
+    <comment ref="AF17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000078000000}">
       <text>
         <r>
           <rPr>
@@ -2083,7 +2089,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK17" authorId="0">
+    <comment ref="AK17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000079000000}">
       <text>
         <r>
           <rPr>
@@ -2102,7 +2108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP17" authorId="0">
+    <comment ref="AP17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007A000000}">
       <text>
         <r>
           <rPr>
@@ -2121,7 +2127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU17" authorId="0">
+    <comment ref="AU17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007B000000}">
       <text>
         <r>
           <rPr>
@@ -2141,7 +2147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V18" authorId="0">
+    <comment ref="V18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007C000000}">
       <text>
         <r>
           <rPr>
@@ -2160,7 +2166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y18" authorId="0">
+    <comment ref="Y18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007D000000}">
       <text>
         <r>
           <rPr>
@@ -2173,7 +2179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA18" authorId="0">
+    <comment ref="AA18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007E000000}">
       <text>
         <r>
           <rPr>
@@ -2196,7 +2202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF18" authorId="0">
+    <comment ref="AF18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007F000000}">
       <text>
         <r>
           <rPr>
@@ -2217,7 +2223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI18" authorId="0">
+    <comment ref="AI18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000080000000}">
       <text>
         <r>
           <rPr>
@@ -2230,7 +2236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V19" authorId="0">
+    <comment ref="V19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000081000000}">
       <text>
         <r>
           <rPr>
@@ -2253,7 +2259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA19" authorId="0">
+    <comment ref="AA19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000082000000}">
       <text>
         <r>
           <rPr>
@@ -2276,7 +2282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF19" authorId="0">
+    <comment ref="AF19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000083000000}">
       <text>
         <r>
           <rPr>
@@ -2297,7 +2303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK19" authorId="0">
+    <comment ref="AK19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000084000000}">
       <text>
         <r>
           <rPr>
@@ -2320,7 +2326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V20" authorId="0">
+    <comment ref="V20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000085000000}">
       <text>
         <r>
           <rPr>
@@ -2340,7 +2346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q21" authorId="0">
+    <comment ref="Q21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000086000000}">
       <text>
         <r>
           <rPr>
@@ -2357,7 +2363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V21" authorId="0">
+    <comment ref="V21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000087000000}">
       <text>
         <r>
           <rPr>
@@ -2384,7 +2390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA21" authorId="0">
+    <comment ref="AA21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000088000000}">
       <text>
         <r>
           <rPr>
@@ -2407,7 +2413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF21" authorId="0">
+    <comment ref="AF21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000089000000}">
       <text>
         <r>
           <rPr>
@@ -2428,7 +2434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK21" authorId="0">
+    <comment ref="AK21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008A000000}">
       <text>
         <r>
           <rPr>
@@ -2455,7 +2461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V22" authorId="0">
+    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008B000000}">
       <text>
         <r>
           <rPr>
@@ -2482,7 +2488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF22" authorId="0">
+    <comment ref="AF22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008C000000}">
       <text>
         <r>
           <rPr>
@@ -2503,7 +2509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q23" authorId="0">
+    <comment ref="Q23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008D000000}">
       <text>
         <r>
           <rPr>
@@ -2525,7 +2531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V23" authorId="0">
+    <comment ref="V23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008E000000}">
       <text>
         <r>
           <rPr>
@@ -2548,7 +2554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF23" authorId="0">
+    <comment ref="AF23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008F000000}">
       <text>
         <r>
           <rPr>
@@ -2569,7 +2575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK23" authorId="0">
+    <comment ref="AK23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000090000000}">
       <text>
         <r>
           <rPr>
@@ -2586,7 +2592,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V24" authorId="0">
+    <comment ref="V24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000091000000}">
       <text>
         <r>
           <rPr>
@@ -2610,7 +2616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA24" authorId="0">
+    <comment ref="AA24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000092000000}">
       <text>
         <r>
           <rPr>
@@ -2632,7 +2638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF24" authorId="0">
+    <comment ref="AF24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000093000000}">
       <text>
         <r>
           <rPr>
@@ -2653,7 +2659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK24" authorId="0">
+    <comment ref="AK24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000094000000}">
       <text>
         <r>
           <rPr>
@@ -2679,7 +2685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q25" authorId="0">
+    <comment ref="Q25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000095000000}">
       <text>
         <r>
           <rPr>
@@ -2701,7 +2707,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V25" authorId="0">
+    <comment ref="V25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000096000000}">
       <text>
         <r>
           <rPr>
@@ -2724,7 +2730,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF25" authorId="0">
+    <comment ref="AF25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000097000000}">
       <text>
         <r>
           <rPr>
@@ -2745,7 +2751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK25" authorId="0">
+    <comment ref="AK25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000098000000}">
       <text>
         <r>
           <rPr>
@@ -2766,7 +2772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q26" authorId="0">
+    <comment ref="Q26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000099000000}">
       <text>
         <r>
           <rPr>
@@ -2786,7 +2792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V26" authorId="0">
+    <comment ref="V26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00009A000000}">
       <text>
         <r>
           <rPr>
@@ -2811,7 +2817,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA26" authorId="0">
+    <comment ref="AA26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00009B000000}">
       <text>
         <r>
           <rPr>
@@ -2835,7 +2841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF26" authorId="0">
+    <comment ref="AF26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00009C000000}">
       <text>
         <r>
           <rPr>
@@ -2856,7 +2862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK26" authorId="0">
+    <comment ref="AK26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00009D000000}">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q27" authorId="0">
+    <comment ref="Q27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00009E000000}">
       <text>
         <r>
           <rPr>
@@ -2902,7 +2908,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V27" authorId="0">
+    <comment ref="V27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00009F000000}">
       <text>
         <r>
           <rPr>
@@ -2927,7 +2933,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF27" authorId="0">
+    <comment ref="AF27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A0000000}">
       <text>
         <r>
           <rPr>
@@ -2948,7 +2954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI27" authorId="0">
+    <comment ref="AI27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A1000000}">
       <text>
         <r>
           <rPr>
@@ -2961,7 +2967,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK27" authorId="0">
+    <comment ref="AK27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A2000000}">
       <text>
         <r>
           <rPr>
@@ -2980,7 +2986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V28" authorId="0">
+    <comment ref="V28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A3000000}">
       <text>
         <r>
           <rPr>
@@ -3005,7 +3011,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF28" authorId="0">
+    <comment ref="AF28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A4000000}">
       <text>
         <r>
           <rPr>
@@ -3026,7 +3032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI28" authorId="0">
+    <comment ref="AI28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A5000000}">
       <text>
         <r>
           <rPr>
@@ -3039,7 +3045,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK28" authorId="0">
+    <comment ref="AK28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A6000000}">
       <text>
         <r>
           <rPr>
@@ -3058,7 +3064,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU28" authorId="0">
+    <comment ref="AU28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A7000000}">
       <text>
         <r>
           <rPr>
@@ -3079,7 +3085,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q29" authorId="0">
+    <comment ref="Q29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A8000000}">
       <text>
         <r>
           <rPr>
@@ -3102,7 +3108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V29" authorId="0">
+    <comment ref="V29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000A9000000}">
       <text>
         <r>
           <rPr>
@@ -3127,7 +3133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF29" authorId="0">
+    <comment ref="AF29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000AA000000}">
       <text>
         <r>
           <rPr>
@@ -3148,7 +3154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI29" authorId="0">
+    <comment ref="AI29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000AB000000}">
       <text>
         <r>
           <rPr>
@@ -3161,7 +3167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK29" authorId="0">
+    <comment ref="AK29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000AC000000}">
       <text>
         <r>
           <rPr>
@@ -3180,7 +3186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU29" authorId="0">
+    <comment ref="AU29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000AD000000}">
       <text>
         <r>
           <rPr>
@@ -3201,7 +3207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q30" authorId="0">
+    <comment ref="Q30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000AE000000}">
       <text>
         <r>
           <rPr>
@@ -3223,7 +3229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V30" authorId="0">
+    <comment ref="V30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000AF000000}">
       <text>
         <r>
           <rPr>
@@ -3248,7 +3254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF30" authorId="0">
+    <comment ref="AF30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B0000000}">
       <text>
         <r>
           <rPr>
@@ -3269,7 +3275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI30" authorId="0">
+    <comment ref="AI30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B1000000}">
       <text>
         <r>
           <rPr>
@@ -3282,7 +3288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK30" authorId="0">
+    <comment ref="AK30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B2000000}">
       <text>
         <r>
           <rPr>
@@ -3301,7 +3307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q31" authorId="0">
+    <comment ref="Q31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B3000000}">
       <text>
         <r>
           <rPr>
@@ -3320,7 +3326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V31" authorId="0">
+    <comment ref="V31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B4000000}">
       <text>
         <r>
           <rPr>
@@ -3343,7 +3349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF31" authorId="0">
+    <comment ref="AF31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B5000000}">
       <text>
         <r>
           <rPr>
@@ -3364,7 +3370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI31" authorId="0">
+    <comment ref="AI31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B6000000}">
       <text>
         <r>
           <rPr>
@@ -3377,7 +3383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK31" authorId="0">
+    <comment ref="AK31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B7000000}">
       <text>
         <r>
           <rPr>
@@ -3394,7 +3400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q32" authorId="0">
+    <comment ref="Q32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B8000000}">
       <text>
         <r>
           <rPr>
@@ -3419,7 +3425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V32" authorId="0">
+    <comment ref="V32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000B9000000}">
       <text>
         <r>
           <rPr>
@@ -3442,7 +3448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF32" authorId="0">
+    <comment ref="AF32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000BA000000}">
       <text>
         <r>
           <rPr>
@@ -3463,7 +3469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK32" authorId="0">
+    <comment ref="AK32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000BB000000}">
       <text>
         <r>
           <rPr>
@@ -3484,7 +3490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M34" authorId="0">
+    <comment ref="M34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000BC000000}">
       <text>
         <r>
           <rPr>
@@ -3497,7 +3503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P34" authorId="0">
+    <comment ref="P34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000BD000000}">
       <text>
         <r>
           <rPr>
@@ -3510,7 +3516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U34" authorId="0">
+    <comment ref="U34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000BE000000}">
       <text>
         <r>
           <rPr>
@@ -3523,7 +3529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z34" authorId="0">
+    <comment ref="Z34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000BF000000}">
       <text>
         <r>
           <rPr>
@@ -3536,7 +3542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE34" authorId="0">
+    <comment ref="AE34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000C0000000}">
       <text>
         <r>
           <rPr>
@@ -3549,7 +3555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ34" authorId="0">
+    <comment ref="AJ34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000C1000000}">
       <text>
         <r>
           <rPr>
@@ -3562,7 +3568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO34" authorId="0">
+    <comment ref="AO34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000C2000000}">
       <text>
         <r>
           <rPr>
@@ -3575,7 +3581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT34" authorId="0">
+    <comment ref="AT34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000C3000000}">
       <text>
         <r>
           <rPr>
@@ -4369,7 +4375,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\€#,##0.00"/>
   </numFmts>
@@ -4563,6 +4569,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4578,15 +4593,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -10454,6 +10460,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -10502,7 +10511,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10535,9 +10544,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10570,6 +10596,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10745,14 +10788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="14" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="14" ySplit="6" topLeftCell="S25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
@@ -10901,71 +10944,71 @@
       </c>
     </row>
     <row r="5" spans="1:49" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="13" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="14" t="s">
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="15" t="s">
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="16" t="s">
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="17" t="s">
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
-      <c r="AL5" s="17"/>
-      <c r="AM5" s="17"/>
-      <c r="AN5" s="18" t="s">
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="AO5" s="18"/>
-      <c r="AP5" s="18"/>
-      <c r="AQ5" s="18"/>
-      <c r="AR5" s="18"/>
-      <c r="AS5" s="19" t="s">
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="AT5" s="19"/>
-      <c r="AU5" s="19"/>
-      <c r="AV5" s="19"/>
-      <c r="AW5" s="19"/>
+      <c r="AT5" s="14"/>
+      <c r="AU5" s="14"/>
+      <c r="AV5" s="14"/>
+      <c r="AW5" s="14"/>
     </row>
     <row r="6" spans="1:49" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
@@ -11164,6 +11207,9 @@
       <c r="T7" s="8">
         <v>93881</v>
       </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
       <c r="V7" s="9">
         <f>IFERROR(LOOKUP(IF(U7="",L7,U7),{0,1,10,25,50,100,250,500,1000,7000},{0,0.52,0.502,0.4928,0.4742,0.4091,0.37192,0.35334,0.27895,0.23668}),"")</f>
         <v>0.52</v>
@@ -11280,6 +11326,9 @@
       <c r="T8" s="11" t="s">
         <v>162</v>
       </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
       <c r="V8" s="9">
         <f>IFERROR(LOOKUP(IF(U8="",L8,U8),{0,1,4000},{0,0.06142,0.06142}),"")</f>
         <v>6.1420000000000002E-2</v>
@@ -11374,6 +11423,9 @@
       <c r="T9" s="8">
         <v>8428569</v>
       </c>
+      <c r="U9">
+        <v>2</v>
+      </c>
       <c r="V9" s="9">
         <f>IFERROR(LOOKUP(IF(U9="",L9,U9),{0,1,10,100,500,1000,4000,8000,12000},{0,0.11,0.08,0.0378,0.02652,0.02195,0.01656,0.01512,0.0144}),"")</f>
         <v>0.11</v>
@@ -11504,6 +11556,9 @@
       <c r="T10" s="8">
         <v>48644</v>
       </c>
+      <c r="U10">
+        <v>2</v>
+      </c>
       <c r="V10" s="9">
         <f>IFERROR(LOOKUP(IF(U10="",L10,U10),{0,1,10,100,500,1000,4000,8000,12000},{0,0.24,0.164,0.0931,0.06568,0.05748,0.0476,0.04522,0.04284}),"")</f>
         <v>0.24</v>
@@ -11592,6 +11647,9 @@
       <c r="T11" s="8">
         <v>212798</v>
       </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
       <c r="V11" s="9">
         <f>IFERROR(LOOKUP(IF(U11="",L11,U11),{0,1,10,100,500,1000,4000,8000,12000},{0,0.1,0.058,0.0255999999999999,0.01832,0.01439,0.01003,0.00916,0.00872}),"")</f>
         <v>0.1</v>
@@ -11680,6 +11738,9 @@
       <c r="T12" s="8">
         <v>47595651</v>
       </c>
+      <c r="U12">
+        <v>9</v>
+      </c>
       <c r="V12" s="9">
         <f>IFERROR(LOOKUP(IF(U12="",L12,U12),{0,1,10,100,500,1000,4000,8000,12000},{0,0.18,0.128,0.06,0.04206,0.03482,0.02578,0.02398,0.02278}),"")</f>
         <v>0.18</v>
@@ -11810,6 +11871,9 @@
       <c r="T13" s="8">
         <v>10000</v>
       </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
       <c r="V13" s="9">
         <f>IFERROR(LOOKUP(IF(U13="",L13,U13),{0,1,10,100,500,1000,10000},{0,0.44,0.374,0.2792,0.21934,0.16949,0.13552}),"")</f>
         <v>0.44</v>
@@ -11884,6 +11948,9 @@
       <c r="T14" s="8">
         <v>1498</v>
       </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
       <c r="V14" s="9">
         <f>IFERROR(LOOKUP(IF(U14="",L14,U14),{0,1,550},{0,3.79999999999999,3.79999999999999}),"")</f>
         <v>3.7999999999999901</v>
@@ -11958,6 +12025,9 @@
       <c r="T15" s="8">
         <v>3052</v>
       </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
       <c r="V15" s="9">
         <f>IFERROR(LOOKUP(IF(U15="",L15,U15),{0,1,50,100,500},{0,11.15,9.6072,8.3418,7.26391999999999}),"")</f>
         <v>11.15</v>
@@ -12060,6 +12130,9 @@
       <c r="T16" s="8">
         <v>34822</v>
       </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
       <c r="V16" s="9">
         <f>IFERROR(LOOKUP(IF(U16="",L16,U16),{0,1,96,192,576,1056},{0,4.87,4.13594,3.58448,3.05141,2.57348}),"")</f>
         <v>4.87</v>
@@ -12176,6 +12249,9 @@
       <c r="T17" s="8">
         <v>13459</v>
       </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
       <c r="V17" s="9">
         <f>IFERROR(LOOKUP(IF(U17="",L17,U17),{0,1,25,100,3000},{0,0.41,0.34,0.309,0.309}),"")</f>
         <v>0.41</v>
@@ -12292,6 +12368,9 @@
       <c r="T18" s="8">
         <v>270</v>
       </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
       <c r="V18" s="9">
         <f>IFERROR(LOOKUP(IF(U18="",L18,U18),{0,1,10,50,100},{0,1.62,1.457,1.377,1.224}),"")</f>
         <v>1.62</v>
@@ -12372,6 +12451,9 @@
       <c r="T19" s="8">
         <v>8226</v>
       </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
       <c r="V19" s="9">
         <f>IFERROR(LOOKUP(IF(U19="",L19,U19),{0,1,10,25,100,250,500,1000,2500},{0,2.98,2.672,2.526,2.1893,2.077,1.86368,1.57177999999999,1.3625}),"")</f>
         <v>2.98</v>
@@ -12460,6 +12542,9 @@
       <c r="T20" s="8">
         <v>401</v>
       </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
       <c r="V20" s="9">
         <f>IFERROR(LOOKUP(IF(U20="",L20,U20),{0,1,25,100,250,500},{0,4.72,3.1324,2.59,2.46052,2.405}),"")</f>
         <v>4.72</v>
@@ -12520,6 +12605,9 @@
       <c r="T21" s="8">
         <v>5450</v>
       </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
       <c r="V21" s="9">
         <f>IFERROR(LOOKUP(IF(U21="",L21,U21),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000},{0,0.47,0.367,0.305599999999999,0.2633,0.23512,0.2022,0.15612,0.14108,0.12825,0.1197,0.11543,0.114}),"")</f>
         <v>0.47</v>
@@ -12608,6 +12696,9 @@
       <c r="T22" s="8">
         <v>5418</v>
       </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
       <c r="V22" s="9">
         <f>IFERROR(LOOKUP(IF(U22="",L22,U22),{0,1,10,25,50,100,250,500,1000,2000,3000,5000,10000},{0,1.05,0.926,0.8712,0.835,0.7986,0.726,0.6534,0.528,0.495,0.4785,0.462,0.4389}),"")</f>
         <v>1.05</v>
@@ -12682,6 +12773,9 @@
       <c r="T23" s="8">
         <v>1942</v>
       </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
       <c r="V23" s="9">
         <f>IFERROR(LOOKUP(IF(U23="",L23,U23),{0,1,10,25,50,100,250,500,1000},{0,4.77,4.543,4.4296,4.3158,4.2023,3.86156,3.0975,2.78775}),"")</f>
         <v>4.7699999999999996</v>
@@ -12756,6 +12850,9 @@
       <c r="T24" s="8">
         <v>16849</v>
       </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
       <c r="V24" s="9">
         <f>IFERROR(LOOKUP(IF(U24="",L24,U24),{0,1,10,100,1000,2500,5000,10000,25000,50000},{0,0.11,0.098,0.0376,0.01654,0.01428,0.01162,0.01042,0.00957,0.00944}),"")</f>
         <v>0.11</v>
@@ -12864,6 +12961,9 @@
       <c r="T25" s="8">
         <v>141618</v>
       </c>
+      <c r="U25">
+        <v>2</v>
+      </c>
       <c r="V25" s="9">
         <f>IFERROR(LOOKUP(IF(U25="",L25,U25),{0,1,10,100,1000,2500,5000,10000,25000},{0,0.1,0.038,0.0156,0.007,0.00607,0.00456,0.00396,0.0036}),"")</f>
         <v>0.1</v>
@@ -12952,6 +13052,9 @@
       <c r="T26" s="8">
         <v>119990</v>
       </c>
+      <c r="U26">
+        <v>2</v>
+      </c>
       <c r="V26" s="9">
         <f>IFERROR(LOOKUP(IF(U26="",L26,U26),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.033,0.0136,0.00609,0.00529,0.00457,0.00397,0.00349,0.00319999999999999,0.00313}),"")</f>
         <v>0.1</v>
@@ -13054,6 +13157,9 @@
       <c r="T27" s="8">
         <v>307334</v>
       </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
       <c r="V27" s="9">
         <f>IFERROR(LOOKUP(IF(U27="",L27,U27),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.042,0.017,0.00762,0.00662,0.00496999999999999,0.00431,0.00379,0.00348,0.00341}),"")</f>
         <v>0.1</v>
@@ -13128,6 +13234,9 @@
       <c r="T28" s="8">
         <v>66537</v>
       </c>
+      <c r="U28">
+        <v>2</v>
+      </c>
       <c r="V28" s="9">
         <f>IFERROR(LOOKUP(IF(U28="",L28,U28),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.042,0.017,0.00762,0.00662,0.00496999999999999,0.00431,0.00379,0.00348,0.00341}),"")</f>
         <v>0.1</v>
@@ -13230,6 +13339,9 @@
       <c r="T29" s="8">
         <v>302269</v>
       </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
       <c r="V29" s="9">
         <f>IFERROR(LOOKUP(IF(U29="",L29,U29),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.042,0.017,0.00762,0.00662,0.00496999999999999,0.00431,0.00379,0.00348,0.00341}),"")</f>
         <v>0.1</v>
@@ -13332,6 +13444,9 @@
       <c r="T30" s="8">
         <v>254536</v>
       </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
       <c r="V30" s="9">
         <f>IFERROR(LOOKUP(IF(U30="",L30,U30),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.042,0.017,0.00762,0.00662,0.00496999999999999,0.00431,0.00379,0.00348,0.00341}),"")</f>
         <v>0.1</v>
@@ -13420,6 +13535,9 @@
       <c r="T31" s="8">
         <v>199199</v>
       </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
       <c r="V31" s="9">
         <f>IFERROR(LOOKUP(IF(U31="",L31,U31),{0,1,10,100,1000,2500,5000,10000,30000},{0,0.1,0.038,0.0156,0.007,0.00607,0.00502,0.00396,0.0036}),"")</f>
         <v>0.1</v>
@@ -13508,6 +13626,9 @@
       <c r="T32" s="8">
         <v>137370</v>
       </c>
+      <c r="U32">
+        <v>3</v>
+      </c>
       <c r="V32" s="9">
         <f>IFERROR(LOOKUP(IF(U32="",L32,U32),{0,1,10,100,1000,2500,5000,10000,25000},{0,0.1,0.038,0.0156,0.007,0.00607,0.00456,0.00396,0.0036}),"")</f>
         <v>0.1</v>
@@ -13557,7 +13678,7 @@
       </c>
       <c r="N34" s="5">
         <f ca="1">SUM(INDIRECT(ADDRESS(ROW(),COLUMN(arrow_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(tme_part_data)+3)))</f>
-        <v>0</v>
+        <v>42.02852</v>
       </c>
       <c r="P34" s="6" t="str">
         <f>IFERROR(IF(OR(P7:P32),COUNTIFS(P7:P32,"&gt;0",R7:R32,"&lt;&gt;")&amp;" of "&amp;(ROWS(R7:R32)-COUNTBLANK(R7:R32))&amp;" parts purchased",""),"")</f>
@@ -13569,11 +13690,11 @@
       </c>
       <c r="U34" s="6" t="str">
         <f>IFERROR(IF(OR(U7:U32),COUNTIFS(U7:U32,"&gt;0",W7:W32,"&lt;&gt;")&amp;" of "&amp;(ROWS(W7:W32)-COUNTBLANK(W7:W32))&amp;" parts purchased",""),"")</f>
-        <v/>
+        <v>26 of 26 parts purchased</v>
       </c>
       <c r="W34" s="5">
         <f>SUMIF(U7:U32,"&gt;0",W7:W32)</f>
-        <v>0</v>
+        <v>42.02852</v>
       </c>
       <c r="Z34" s="6" t="str">
         <f>IFERROR(IF(OR(Z7:Z32),COUNTIFS(Z7:Z32,"&gt;0",AB7:AB32,"&lt;&gt;")&amp;" of "&amp;(ROWS(AB7:AB32)-COUNTBLANK(AB7:AB32))&amp;" parts purchased",""),"")</f>
@@ -13623,7 +13744,7 @@
       </c>
       <c r="U35" t="str">
         <f t="array" ref="U35">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,401-1427-1-ND,BOOT1;EN1</v>
       </c>
       <c r="Z35" t="str">
         <f t="array" ref="Z35">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13653,7 +13774,7 @@
       </c>
       <c r="U36" t="str">
         <f t="array" ref="U36">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>6,490-3340-2-ND,C1;C2;C5;C6;C16;C18</v>
       </c>
       <c r="Z36" t="str">
         <f t="array" ref="Z36">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13683,7 +13804,7 @@
       </c>
       <c r="U37" t="str">
         <f t="array" ref="U37">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,311-1136-1-ND,C10;C12</v>
       </c>
       <c r="Z37" t="str">
         <f t="array" ref="Z37">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13713,7 +13834,7 @@
       </c>
       <c r="U38" t="str">
         <f t="array" ref="U38">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,399-16641-1-ND,C20;C21</v>
       </c>
       <c r="Z38" t="str">
         <f t="array" ref="Z38">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13743,7 +13864,7 @@
       </c>
       <c r="U39" t="str">
         <f t="array" ref="U39">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,1276-1300-1-ND,C3;C4</v>
       </c>
       <c r="Z39" t="str">
         <f t="array" ref="Z39">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13773,7 +13894,7 @@
       </c>
       <c r="U40" t="str">
         <f t="array" ref="U40">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>9,478-1395-1-ND,C7-C9;C11;C13-C15;C17;C19</v>
       </c>
       <c r="Z40" t="str">
         <f t="array" ref="Z40">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13803,7 +13924,7 @@
       </c>
       <c r="U41" t="str">
         <f t="array" ref="U41">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,497-18870-1-ND,D7</v>
       </c>
       <c r="Z41" t="str">
         <f t="array" ref="Z41">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13833,7 +13954,7 @@
       </c>
       <c r="U42" t="str">
         <f t="array" ref="U42">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,1904-1010-1-ND,IC1</v>
       </c>
       <c r="Z42" t="str">
         <f t="array" ref="Z42">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13863,7 +13984,7 @@
       </c>
       <c r="U43" t="str">
         <f t="array" ref="U43">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,AD5667RBRMZ-2-ND,IC2</v>
       </c>
       <c r="Z43" t="str">
         <f t="array" ref="Z43">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13893,7 +14014,7 @@
       </c>
       <c r="U44" t="str">
         <f t="array" ref="U44">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,AD8608ARUZ-ND,IC3</v>
       </c>
       <c r="Z44" t="str">
         <f t="array" ref="Z44">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13923,7 +14044,7 @@
       </c>
       <c r="U45" t="str">
         <f t="array" ref="U45">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,576-1259-1-ND,IC4;IC5</v>
       </c>
       <c r="Z45" t="str">
         <f t="array" ref="Z45">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13953,7 +14074,7 @@
       </c>
       <c r="U46" t="str">
         <f t="array" ref="U46">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,MAX4643EUA+-ND,IC6</v>
       </c>
       <c r="Z46" t="str">
         <f t="array" ref="Z46">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -13983,7 +14104,7 @@
       </c>
       <c r="U47" t="str">
         <f t="array" ref="U47">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,MAX4644EUT+TCT-ND,IC7</v>
       </c>
       <c r="Z47" t="str">
         <f t="array" ref="Z47">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14013,7 +14134,7 @@
       </c>
       <c r="U48" t="str">
         <f t="array" ref="U48">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,LTC2471IMS#PBF-ND,IC8</v>
       </c>
       <c r="Z48" t="str">
         <f t="array" ref="Z48">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14043,7 +14164,7 @@
       </c>
       <c r="U49" t="str">
         <f t="array" ref="U49">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,VAOL-S8SB4CT-ND,LED1</v>
       </c>
       <c r="Z49" t="str">
         <f t="array" ref="Z49">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14073,7 +14194,7 @@
       </c>
       <c r="U50" t="str">
         <f t="array" ref="U50">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,CP-032HPJCT-ND,P1</v>
       </c>
       <c r="Z50" t="str">
         <f t="array" ref="Z50">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14103,7 +14224,7 @@
       </c>
       <c r="U51" t="str">
         <f t="array" ref="U51">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,GH7540CT-ND,P2</v>
       </c>
       <c r="Z51" t="str">
         <f t="array" ref="Z51">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14133,7 +14254,7 @@
       </c>
       <c r="U52" t="str">
         <f t="array" ref="U52">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,RR12P1.2KDCT-ND,R1</v>
       </c>
       <c r="Z52" t="str">
         <f t="array" ref="Z52">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14163,7 +14284,7 @@
       </c>
       <c r="U53" t="str">
         <f t="array" ref="U53">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,541-4163-1-ND,R11;R12</v>
       </c>
       <c r="Z53" t="str">
         <f t="array" ref="Z53">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14193,7 +14314,7 @@
       </c>
       <c r="U54" t="str">
         <f t="array" ref="U54">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,A130132CT-ND,R14;R15</v>
       </c>
       <c r="Z54" t="str">
         <f t="array" ref="Z54">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14223,7 +14344,7 @@
       </c>
       <c r="U55" t="str">
         <f t="array" ref="U55">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,311-16.2KCRCT-ND,R2</v>
       </c>
       <c r="Z55" t="str">
         <f t="array" ref="Z55">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14253,7 +14374,7 @@
       </c>
       <c r="U56" t="str">
         <f t="array" ref="U56">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>2,311-845CRCT-ND,R3;R10</v>
       </c>
       <c r="Z56" t="str">
         <f t="array" ref="Z56">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14283,7 +14404,7 @@
       </c>
       <c r="U57" t="str">
         <f t="array" ref="U57">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,311-29.4KCRCT-ND,R4</v>
       </c>
       <c r="Z57" t="str">
         <f t="array" ref="Z57">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14313,7 +14434,7 @@
       </c>
       <c r="U58" t="str">
         <f t="array" ref="U58">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,311-8.06KCRCT-ND,R5</v>
       </c>
       <c r="Z58" t="str">
         <f t="array" ref="Z58">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14343,7 +14464,7 @@
       </c>
       <c r="U59" t="str">
         <f t="array" ref="U59">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>1,541-4126-1-ND,R7</v>
       </c>
       <c r="Z59" t="str">
         <f t="array" ref="Z59">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -14373,7 +14494,7 @@
       </c>
       <c r="U60" t="str">
         <f t="array" ref="U60">IFERROR(CONCATENATE(TEXT(INDEX(U7:U32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),"##0"),",",INDEX(X7:X32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(U7:U32),IF(U7:U32&gt;0,IF(X7:X32&lt;&gt;"",ROW(U7:U32)-MIN(ROW(U7:U32))+1))),ROW()-ROW(A$35)+1)),",",";")),"")</f>
-        <v/>
+        <v>3,541-4164-1-ND,R8;R9;R13</v>
       </c>
       <c r="Z60" t="str">
         <f t="array" ref="Z60">IFERROR(CONCATENATE(INDEX(AC7:AC32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",TEXT(INDEX(Z7:Z32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1)),"##0")," ",SUBSTITUTE(INDEX(A7:A32,SMALL(IF(ISNUMBER(Z7:Z32),IF(Z7:Z32&gt;0,IF(AC7:AC32&lt;&gt;"",ROW(Z7:Z32)-MIN(ROW(Z7:Z32))+1))),ROW()-ROW(A$35)+1))," ",";")),"")</f>
@@ -17371,147 +17492,147 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="K7" r:id="rId1"/>
-    <hyperlink ref="S7" r:id="rId2"/>
-    <hyperlink ref="X7" r:id="rId3"/>
-    <hyperlink ref="AC7" r:id="rId4"/>
-    <hyperlink ref="AH7" r:id="rId5"/>
-    <hyperlink ref="AM7" r:id="rId6"/>
-    <hyperlink ref="AR7" r:id="rId7"/>
-    <hyperlink ref="K8" r:id="rId8"/>
-    <hyperlink ref="S8" r:id="rId9"/>
-    <hyperlink ref="X8" r:id="rId10"/>
-    <hyperlink ref="AC8" r:id="rId11"/>
-    <hyperlink ref="AM8" r:id="rId12"/>
-    <hyperlink ref="AW8" r:id="rId13"/>
-    <hyperlink ref="K9" r:id="rId14"/>
-    <hyperlink ref="S9" r:id="rId15"/>
-    <hyperlink ref="X9" r:id="rId16"/>
-    <hyperlink ref="AC9" r:id="rId17"/>
-    <hyperlink ref="AH9" r:id="rId18"/>
-    <hyperlink ref="AM9" r:id="rId19"/>
-    <hyperlink ref="AR9" r:id="rId20"/>
-    <hyperlink ref="AW9" r:id="rId21"/>
-    <hyperlink ref="K10" r:id="rId22"/>
-    <hyperlink ref="S10" r:id="rId23"/>
-    <hyperlink ref="X10" r:id="rId24"/>
-    <hyperlink ref="AC10" r:id="rId25"/>
-    <hyperlink ref="AH10" r:id="rId26"/>
-    <hyperlink ref="K11" r:id="rId27"/>
-    <hyperlink ref="S11" r:id="rId28"/>
-    <hyperlink ref="X11" r:id="rId29"/>
-    <hyperlink ref="AR11" r:id="rId30"/>
-    <hyperlink ref="AW11" r:id="rId31"/>
-    <hyperlink ref="K12" r:id="rId32"/>
-    <hyperlink ref="S12" r:id="rId33"/>
-    <hyperlink ref="X12" r:id="rId34"/>
-    <hyperlink ref="AC12" r:id="rId35"/>
-    <hyperlink ref="AH12" r:id="rId36"/>
-    <hyperlink ref="AM12" r:id="rId37"/>
-    <hyperlink ref="AR12" r:id="rId38"/>
-    <hyperlink ref="AW12" r:id="rId39"/>
-    <hyperlink ref="K13" r:id="rId40"/>
-    <hyperlink ref="S13" r:id="rId41"/>
-    <hyperlink ref="X13" r:id="rId42"/>
-    <hyperlink ref="AH13" r:id="rId43"/>
-    <hyperlink ref="AM13" r:id="rId44"/>
-    <hyperlink ref="K14" r:id="rId45"/>
-    <hyperlink ref="X14" r:id="rId46"/>
-    <hyperlink ref="AH14" r:id="rId47"/>
-    <hyperlink ref="K15" r:id="rId48"/>
-    <hyperlink ref="S15" r:id="rId49"/>
-    <hyperlink ref="X15" r:id="rId50"/>
-    <hyperlink ref="AC15" r:id="rId51"/>
-    <hyperlink ref="AH15" r:id="rId52"/>
-    <hyperlink ref="AR15" r:id="rId53"/>
-    <hyperlink ref="K16" r:id="rId54"/>
-    <hyperlink ref="S16" r:id="rId55"/>
-    <hyperlink ref="X16" r:id="rId56"/>
-    <hyperlink ref="AC16" r:id="rId57"/>
-    <hyperlink ref="AH16" r:id="rId58"/>
-    <hyperlink ref="AR16" r:id="rId59"/>
-    <hyperlink ref="AW16" r:id="rId60"/>
-    <hyperlink ref="K17" r:id="rId61"/>
-    <hyperlink ref="S17" r:id="rId62"/>
-    <hyperlink ref="X17" r:id="rId63"/>
-    <hyperlink ref="AC17" r:id="rId64"/>
-    <hyperlink ref="AH17" r:id="rId65"/>
-    <hyperlink ref="AM17" r:id="rId66"/>
-    <hyperlink ref="AR17" r:id="rId67"/>
-    <hyperlink ref="AW17" r:id="rId68"/>
-    <hyperlink ref="K18" r:id="rId69"/>
-    <hyperlink ref="X18" r:id="rId70"/>
-    <hyperlink ref="AC18" r:id="rId71"/>
-    <hyperlink ref="AH18" r:id="rId72"/>
-    <hyperlink ref="AM18" r:id="rId73"/>
-    <hyperlink ref="K19" r:id="rId74"/>
-    <hyperlink ref="X19" r:id="rId75"/>
-    <hyperlink ref="AC19" r:id="rId76"/>
-    <hyperlink ref="AH19" r:id="rId77"/>
-    <hyperlink ref="AM19" r:id="rId78"/>
-    <hyperlink ref="K20" r:id="rId79"/>
-    <hyperlink ref="X20" r:id="rId80"/>
-    <hyperlink ref="K21" r:id="rId81"/>
-    <hyperlink ref="S21" r:id="rId82"/>
-    <hyperlink ref="X21" r:id="rId83"/>
-    <hyperlink ref="AC21" r:id="rId84"/>
-    <hyperlink ref="AH21" r:id="rId85"/>
-    <hyperlink ref="AM21" r:id="rId86"/>
-    <hyperlink ref="K22" r:id="rId87"/>
-    <hyperlink ref="X22" r:id="rId88"/>
-    <hyperlink ref="AH22" r:id="rId89"/>
-    <hyperlink ref="K23" r:id="rId90"/>
-    <hyperlink ref="S23" r:id="rId91"/>
-    <hyperlink ref="X23" r:id="rId92"/>
-    <hyperlink ref="AH23" r:id="rId93"/>
-    <hyperlink ref="AM23" r:id="rId94"/>
-    <hyperlink ref="K24" r:id="rId95"/>
-    <hyperlink ref="X24" r:id="rId96"/>
-    <hyperlink ref="AC24" r:id="rId97"/>
-    <hyperlink ref="AH24" r:id="rId98"/>
-    <hyperlink ref="AM24" r:id="rId99"/>
-    <hyperlink ref="AR24" r:id="rId100"/>
-    <hyperlink ref="S25" r:id="rId101"/>
-    <hyperlink ref="X25" r:id="rId102"/>
-    <hyperlink ref="AH25" r:id="rId103"/>
-    <hyperlink ref="AM25" r:id="rId104"/>
-    <hyperlink ref="K26" r:id="rId105"/>
-    <hyperlink ref="S26" r:id="rId106"/>
-    <hyperlink ref="X26" r:id="rId107"/>
-    <hyperlink ref="AC26" r:id="rId108"/>
-    <hyperlink ref="AH26" r:id="rId109"/>
-    <hyperlink ref="AM26" r:id="rId110"/>
-    <hyperlink ref="K27" r:id="rId111"/>
-    <hyperlink ref="S27" r:id="rId112"/>
-    <hyperlink ref="X27" r:id="rId113"/>
-    <hyperlink ref="AH27" r:id="rId114"/>
-    <hyperlink ref="AM27" r:id="rId115"/>
-    <hyperlink ref="K28" r:id="rId116"/>
-    <hyperlink ref="X28" r:id="rId117"/>
-    <hyperlink ref="AH28" r:id="rId118"/>
-    <hyperlink ref="AM28" r:id="rId119"/>
-    <hyperlink ref="AW28" r:id="rId120"/>
-    <hyperlink ref="K29" r:id="rId121"/>
-    <hyperlink ref="S29" r:id="rId122"/>
-    <hyperlink ref="X29" r:id="rId123"/>
-    <hyperlink ref="AH29" r:id="rId124"/>
-    <hyperlink ref="AM29" r:id="rId125"/>
-    <hyperlink ref="AW29" r:id="rId126"/>
-    <hyperlink ref="K30" r:id="rId127"/>
-    <hyperlink ref="S30" r:id="rId128"/>
-    <hyperlink ref="X30" r:id="rId129"/>
-    <hyperlink ref="AH30" r:id="rId130"/>
-    <hyperlink ref="AM30" r:id="rId131"/>
-    <hyperlink ref="K31" r:id="rId132"/>
-    <hyperlink ref="S31" r:id="rId133"/>
-    <hyperlink ref="X31" r:id="rId134"/>
-    <hyperlink ref="AH31" r:id="rId135"/>
-    <hyperlink ref="AM31" r:id="rId136"/>
-    <hyperlink ref="K32" r:id="rId137"/>
-    <hyperlink ref="S32" r:id="rId138"/>
-    <hyperlink ref="X32" r:id="rId139"/>
-    <hyperlink ref="AH32" r:id="rId140"/>
-    <hyperlink ref="AM32" r:id="rId141"/>
+    <hyperlink ref="K7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="S7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="X7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AC7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="AH7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="AM7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="AR7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="S8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="X8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="AC8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="AM8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="AW8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="S9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="X9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="AC9" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="AH9" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="AM9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="AR9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="AW9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="K10" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="S10" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="X10" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="AC10" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="AH10" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="K11" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="S11" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="X11" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="AR11" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="AW11" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K12" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="S12" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="X12" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="AC12" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="AH12" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="AM12" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="AR12" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="AW12" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="K13" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="S13" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="X13" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="AH13" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="AM13" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="K14" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="X14" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="AH14" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="K15" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="S15" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="X15" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="AC15" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="AH15" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="AR15" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="K16" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="S16" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="X16" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="AC16" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="AH16" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="AR16" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="AW16" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="K17" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="S17" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="X17" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="AC17" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="AH17" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="AM17" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="AR17" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="AW17" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="K18" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="X18" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="AC18" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="AH18" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="AM18" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="K19" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="X19" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="AC19" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="AH19" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="AM19" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="K20" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="X20" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="K21" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="S21" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="X21" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="AC21" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="AH21" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="AM21" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="K22" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="X22" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="AH22" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="K23" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="S23" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="X23" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="AH23" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="AM23" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="K24" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="X24" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="AC24" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="AH24" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="AM24" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="AR24" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="S25" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="X25" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="AH25" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="AM25" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="K26" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="S26" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="X26" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="AC26" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="AH26" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="AM26" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="K27" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="S27" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="X27" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="AH27" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="AM27" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="K28" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="X28" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="AH28" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="AM28" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="AW28" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="K29" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="S29" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="X29" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="AH29" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="AM29" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="AW29" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="K30" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="S30" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="X30" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="AH30" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="AM30" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="K31" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="S31" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="X31" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="AH31" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="AM31" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="K32" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="S32" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="X32" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="AH32" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="AM32" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId142"/>

</xml_diff>